<commit_message>
add data preprocessing code
</commit_message>
<xml_diff>
--- a/data/lander_test/shift_requirements.xlsx
+++ b/data/lander_test/shift_requirements.xlsx
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Shift 1</t>
+          <t>Primary Shift</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Shift 2</t>
+          <t>Secondary Shift</t>
         </is>
       </c>
     </row>

</xml_diff>